<commit_message>
excel true positive data update
</commit_message>
<xml_diff>
--- a/RLTesting/logs/bug library.xlsx
+++ b/RLTesting/logs/bug library.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkson\research\SB3 TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkson\research\SB3 TEST\stable-baselines3-testing-new\RLTesting\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBEF9A3-CD79-4517-BAB4-38E371B74A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6639AB5B-291C-4EEF-B478-D07FCB21C1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="66">
   <si>
     <t>Testbed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -301,12 +312,24 @@
     <t>Number of zero-convergence-break events</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Learn result\Actual result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +369,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -367,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -375,6 +404,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -655,19 +685,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P70"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.4140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="41.08203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.4140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="49.08203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.25" style="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="1" customWidth="1"/>
@@ -677,8 +707,9 @@
     <col min="12" max="12" width="27.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="30.25" style="1" customWidth="1"/>
     <col min="14" max="15" width="30.25" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="14.75" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.6640625" style="1"/>
+    <col min="16" max="16" width="16.9140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.08203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -3058,9 +3089,7 @@
       <c r="E67" s="1">
         <v>6</v>
       </c>
-      <c r="O67" s="3">
-        <v>0.828125</v>
-      </c>
+      <c r="O67" s="3"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
@@ -3078,9 +3107,7 @@
       <c r="E68" s="1">
         <v>9</v>
       </c>
-      <c r="O68" s="3">
-        <v>5.46875E-2</v>
-      </c>
+      <c r="O68" s="3"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
@@ -3115,8 +3142,85 @@
       <c r="E70" s="1">
         <v>9</v>
       </c>
-      <c r="O70" s="3">
+      <c r="O70" s="3"/>
+    </row>
+    <row r="78" spans="1:15" ht="15" x14ac:dyDescent="0.4">
+      <c r="C78" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C79" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D79" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="E79" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C80" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1">
+        <f>COUNTIF(M2:M57,"&gt;7")</f>
+        <v>33</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C81" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1">
+        <f>COUNTIF(M2:M57,"&lt;= 7")</f>
+        <v>23</v>
+      </c>
+      <c r="E81" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C90" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D91" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C92" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D92" s="1">
+        <f>COUNTIF(M2:M57,"&gt;6")</f>
+        <v>36</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1">
+        <v>20</v>
+      </c>
+      <c r="E93" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Chapter4 analysis part
</commit_message>
<xml_diff>
--- a/RLTesting/logs/bug library.xlsx
+++ b/RLTesting/logs/bug library.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\research\shiyu\RL-testing-new\RLTesting\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangshiyu/Documents/GitHub/RL-testing-new-2/RLTesting/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6073176E-4A9E-4BAD-8976-018D97049B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043ED617-B57A-E643-8B8B-11966B360380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12720" yWindow="500" windowWidth="22980" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="84">
   <si>
     <t>Testbed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -359,22 +360,49 @@
     <t>Exploring the enviroment</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Fuzzy Oracle Positive Result</t>
+  </si>
+  <si>
+    <t>Human Oracle Positive Result</t>
+  </si>
+  <si>
+    <t>Fuzzy Oracle Positive Rate</t>
+  </si>
+  <si>
+    <t>Human Oracle Positive Rate</t>
+  </si>
+  <si>
+    <t>Frozen Lake</t>
+  </si>
+  <si>
+    <t>DQN</t>
+  </si>
+  <si>
+    <t>PPO</t>
+  </si>
+  <si>
+    <t>Mountaincar Continuous</t>
+  </si>
+  <si>
+    <t>bug-free</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -410,6 +438,18 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -431,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -440,9 +480,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -722,32 +764,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E57"/>
+    <sheetView topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="20.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="41.08203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="41" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="49.08203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.58203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="26.83203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="27.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="30.25" style="1" customWidth="1"/>
-    <col min="15" max="16" width="30.25" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.9140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="17.08203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.1640625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="30.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17" style="1" customWidth="1"/>
     <col min="19" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -800,7 +842,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -844,7 +886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="15">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -888,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -932,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -976,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="15">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1020,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="15">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1064,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="15">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1108,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1152,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="15">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1196,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="15">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1284,7 +1326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="15">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -1325,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="15">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1369,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="15">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1413,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="15">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1457,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="15">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1501,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="15">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="15">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1589,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="15">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1633,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="15">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1677,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="15">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1721,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="15">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1765,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="15">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1809,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="15">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1853,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="15">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1897,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="15">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1941,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="15">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1985,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="15">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -2029,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="15">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -2073,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="15">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -2117,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="15">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -2161,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="15">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2205,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="15">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -2249,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" ht="15">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
@@ -2293,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" ht="15">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
@@ -2337,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" ht="15">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -2381,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="15">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
@@ -2425,7 +2467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="15">
       <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
@@ -2469,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="15">
       <c r="A40" s="1" t="s">
         <v>51</v>
       </c>
@@ -2513,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="15">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
@@ -2557,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="15">
       <c r="A42" s="1" t="s">
         <v>51</v>
       </c>
@@ -2601,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="15">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -2645,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="15">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -2689,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="15">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -2733,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="15">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -2777,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="15">
       <c r="A47" s="1" t="s">
         <v>51</v>
       </c>
@@ -2821,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="15">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -2865,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="15">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
@@ -2909,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="15">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -2953,7 +2995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="15">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
@@ -2997,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" ht="15">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -3041,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="15">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -3085,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" ht="15">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
@@ -3129,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="15">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -3173,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="15">
       <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
@@ -3217,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="15">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
@@ -3261,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16">
       <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
@@ -3279,7 +3321,7 @@
       </c>
       <c r="P66" s="3"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16">
       <c r="A67" s="1" t="s">
         <v>8</v>
       </c>
@@ -3297,7 +3339,7 @@
       </c>
       <c r="P67" s="3"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16">
       <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
@@ -3315,7 +3357,7 @@
       </c>
       <c r="P68" s="3"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16">
       <c r="A69" s="1" t="s">
         <v>51</v>
       </c>
@@ -3332,7 +3374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16">
       <c r="A70" s="1" t="s">
         <v>51</v>
       </c>
@@ -3350,12 +3392,12 @@
       </c>
       <c r="P70" s="3"/>
     </row>
-    <row r="78" spans="1:16" ht="15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:16" ht="15">
       <c r="C78" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16">
       <c r="C79" s="1" t="s">
         <v>63</v>
       </c>
@@ -3366,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16">
       <c r="C80" s="1" t="b">
         <v>1</v>
       </c>
@@ -3378,7 +3420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:6">
       <c r="C81" s="1" t="b">
         <v>0</v>
       </c>
@@ -3390,12 +3432,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:6">
       <c r="C90" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:6">
       <c r="C91" s="1" t="s">
         <v>63</v>
       </c>
@@ -3406,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:6">
       <c r="C92" s="1" t="b">
         <v>1</v>
       </c>
@@ -3418,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:6">
       <c r="C93" s="1" t="b">
         <v>0</v>
       </c>
@@ -3434,4 +3476,2046 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE85A936-484C-9247-9590-E6537AEF2450}">
+  <dimension ref="A1:J62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1">
+        <f>H2/10</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>10</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>I2/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1">
+        <f>H3/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H3" s="6">
+        <v>9</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f>I3/5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1">
+        <f>H4/10</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>10</v>
+      </c>
+      <c r="I4" s="7">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <f>I4/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1">
+        <f>H5/10</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f>I5/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1">
+        <f>H6/10</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>10</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f>I6/5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1">
+        <f>H7/10</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <f>I7/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1">
+        <f>H8/10</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>10</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>I8/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1">
+        <f>H9/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H9" s="6">
+        <v>9</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>I9/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1">
+        <f>H10/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H10" s="6">
+        <v>9</v>
+      </c>
+      <c r="I10" s="7">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <f>I10/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1">
+        <f>H11/10</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <f>I11/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1">
+        <f>H12/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="6">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f>I12/5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1">
+        <f>H13/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H13" s="6">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <f>I13/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1">
+        <f>H14/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="H14" s="6">
+        <v>7</v>
+      </c>
+      <c r="I14" s="7">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <f>I14/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1">
+        <f>H15/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H15" s="6">
+        <v>9</v>
+      </c>
+      <c r="I15" s="7">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <f>I15/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1">
+        <f>H16/10</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="6">
+        <v>10</v>
+      </c>
+      <c r="I16" s="7">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <f>I16/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1">
+        <f>H17/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="H17" s="6">
+        <v>6</v>
+      </c>
+      <c r="I17" s="7">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f>I17/5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1">
+        <f>H18/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H18" s="6">
+        <v>9</v>
+      </c>
+      <c r="I18" s="7">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <f>I18/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="1">
+        <f>H19/10</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="6">
+        <v>10</v>
+      </c>
+      <c r="I19" s="7">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <f>I19/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="1">
+        <f>H20/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="H20" s="6">
+        <v>6</v>
+      </c>
+      <c r="I20" s="7">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <f>I20/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="1">
+        <f>H21/10</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="6">
+        <v>10</v>
+      </c>
+      <c r="I21" s="7">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <f>I21/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="1">
+        <f>H22/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="H22" s="6">
+        <v>4</v>
+      </c>
+      <c r="I22" s="7">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <f>I22/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1">
+        <f>H23/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="H23" s="6">
+        <v>6</v>
+      </c>
+      <c r="I23" s="7">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <f>I23/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1">
+        <v>22</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1">
+        <f>H24/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="H24" s="6">
+        <v>4</v>
+      </c>
+      <c r="I24" s="7">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <f>I24/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="1">
+        <v>23</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1">
+        <f>H25/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="6">
+        <v>5</v>
+      </c>
+      <c r="I25" s="7">
+        <v>5</v>
+      </c>
+      <c r="J25">
+        <f>I25/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1">
+        <v>7</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="1">
+        <f>H26/10</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="6">
+        <v>10</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>I26/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="1">
+        <f>H27/10</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="6">
+        <v>10</v>
+      </c>
+      <c r="I27" s="7">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <f>I27/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1">
+        <v>26</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="1">
+        <f>H28/10</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="6">
+        <v>10</v>
+      </c>
+      <c r="I28" s="7">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <f>I28/5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="1">
+        <f>H29/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H29" s="6">
+        <v>9</v>
+      </c>
+      <c r="I29" s="7">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <f>I29/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1">
+        <v>28</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="1">
+        <f>H30/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H30" s="6">
+        <v>9</v>
+      </c>
+      <c r="I30" s="7">
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <f>I30/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1">
+        <v>33</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="1">
+        <f>H31/10</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="6">
+        <v>10</v>
+      </c>
+      <c r="I31" s="7">
+        <v>5</v>
+      </c>
+      <c r="J31">
+        <f>I31/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="1">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="1">
+        <f>H32/10</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="6">
+        <v>10</v>
+      </c>
+      <c r="I32" s="7">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f>I32/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1">
+        <f>H33/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H33" s="6">
+        <v>9</v>
+      </c>
+      <c r="I33" s="7">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <f>I33/5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="1">
+        <v>36</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="1">
+        <f>H34/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H34" s="6">
+        <v>9</v>
+      </c>
+      <c r="I34" s="7">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f>I34/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1">
+        <v>37</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="1">
+        <f>H35/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H35" s="6">
+        <v>9</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f>I35/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1">
+        <v>38</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="1">
+        <f>H36/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H36" s="6">
+        <v>9</v>
+      </c>
+      <c r="I36" s="7">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f>I36/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1">
+        <v>39</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="1">
+        <f>H37/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="H37" s="6">
+        <v>5</v>
+      </c>
+      <c r="I37" s="7">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <f>I37/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1">
+        <v>24</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1">
+        <f>H38/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="H38" s="6">
+        <v>5</v>
+      </c>
+      <c r="I38" s="7">
+        <v>4</v>
+      </c>
+      <c r="J38">
+        <f>I38/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="1">
+        <f>H39/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H39" s="6">
+        <v>8</v>
+      </c>
+      <c r="I39" s="7">
+        <v>3</v>
+      </c>
+      <c r="J39">
+        <f>I39/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1">
+        <v>26</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="1">
+        <f>H40/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="H40" s="6">
+        <v>1</v>
+      </c>
+      <c r="I40" s="7">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <f>I40/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="1">
+        <v>27</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="1">
+        <f>H41/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="H41" s="6">
+        <v>4</v>
+      </c>
+      <c r="I41" s="7">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <f>I41/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1">
+        <v>28</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="1">
+        <f>H42/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="H42" s="6">
+        <v>6</v>
+      </c>
+      <c r="I42" s="7">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <f>I42/5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1">
+        <v>29</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="1">
+        <f>H43/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="H43" s="6">
+        <v>5</v>
+      </c>
+      <c r="I43" s="7">
+        <v>4</v>
+      </c>
+      <c r="J43">
+        <f>I43/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="1">
+        <v>30</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="1">
+        <f>H44/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="H44" s="6">
+        <v>3</v>
+      </c>
+      <c r="I44" s="7">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <f>I44/5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1">
+        <v>31</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="1">
+        <f>H45/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="H45" s="6">
+        <v>4</v>
+      </c>
+      <c r="I45" s="7">
+        <v>4</v>
+      </c>
+      <c r="J45">
+        <f>I45/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1">
+        <v>32</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="1">
+        <f>H46/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="H46" s="6">
+        <v>4</v>
+      </c>
+      <c r="I46" s="7">
+        <v>4</v>
+      </c>
+      <c r="J46">
+        <f>I46/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1">
+        <v>25</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="1">
+        <f>H47/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H47" s="6">
+        <v>9</v>
+      </c>
+      <c r="I47" s="7">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <f>I47/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1">
+        <v>26</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="1">
+        <f>H48/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H48" s="6">
+        <v>8</v>
+      </c>
+      <c r="I48" s="7">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <f>I48/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="1">
+        <v>27</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="1">
+        <f>H49/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="H49" s="6">
+        <v>2</v>
+      </c>
+      <c r="I49" s="7">
+        <v>5</v>
+      </c>
+      <c r="J49">
+        <f>I49/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="1">
+        <v>28</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="1">
+        <f>H50/10</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="6">
+        <v>10</v>
+      </c>
+      <c r="I50" s="7">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <f>I50/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1">
+        <v>33</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="1">
+        <f>H51/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="H51" s="6">
+        <v>7</v>
+      </c>
+      <c r="I51" s="7">
+        <v>5</v>
+      </c>
+      <c r="J51">
+        <f>I51/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="1">
+        <v>34</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="1">
+        <f>H52/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H52" s="6">
+        <v>8</v>
+      </c>
+      <c r="I52" s="7">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <f>I52/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1">
+        <v>35</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="1">
+        <f>H53/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="H53" s="6">
+        <v>9</v>
+      </c>
+      <c r="I53" s="7">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <f>I53/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="1">
+        <v>36</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="1">
+        <f>H54/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="H54" s="6">
+        <v>7</v>
+      </c>
+      <c r="I54" s="7">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <f>I54/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="1">
+        <v>37</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="1">
+        <f>H55/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H55" s="6">
+        <v>8</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <f>I55/5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="1">
+        <v>38</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" s="1">
+        <f>H56/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="H56" s="6">
+        <v>8</v>
+      </c>
+      <c r="I56" s="7">
+        <v>3</v>
+      </c>
+      <c r="J56">
+        <f>I56/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="1">
+        <v>39</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" s="1">
+        <f>H57/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="H57" s="6">
+        <v>4</v>
+      </c>
+      <c r="I57" s="7">
+        <v>5</v>
+      </c>
+      <c r="J57">
+        <f>I57/5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>83</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" t="s">
+        <v>83</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J59">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" t="s">
+        <v>83</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>83</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J61">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>